<commit_message>
mobile banking vendors updated
</commit_message>
<xml_diff>
--- a/03_UE1_Anbieterevaluierung.xlsx
+++ b/03_UE1_Anbieterevaluierung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="715" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="715"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile Banking" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="174">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -131,9 +131,6 @@
     <t>Support/Hotline</t>
   </si>
   <si>
-    <t>Shortlist</t>
-  </si>
-  <si>
     <t>Maestro</t>
   </si>
   <si>
@@ -537,13 +534,34 @@
   </si>
   <si>
     <t>Nein/Ja</t>
+  </si>
+  <si>
+    <t>iOS/Android</t>
+  </si>
+  <si>
+    <t>iOS/Android/Blackberry/Windows</t>
+  </si>
+  <si>
+    <t>iOS/Android/Blackberry</t>
+  </si>
+  <si>
+    <t>iOs/Android/Blackberry</t>
+  </si>
+  <si>
+    <t>iOS/Android/Blackbery/Windows</t>
+  </si>
+  <si>
+    <t>$ 51.1 Mil.</t>
+  </si>
+  <si>
+    <t>$ 606 Mil.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,7 +666,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,9 +679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -701,7 +719,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -735,7 +753,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -770,10 +787,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -946,19 +962,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C31" sqref="C31"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" style="9" customWidth="1"/>
@@ -970,14 +986,13 @@
     <col min="8" max="8" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="48" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1009,36 +1024,33 @@
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
       </c>
       <c r="F2" s="3">
         <v>750</v>
@@ -1052,33 +1064,32 @@
       <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
       </c>
       <c r="F3" s="3">
         <v>30000</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>7</v>
@@ -1089,33 +1100,37 @@
       <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="M3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
       </c>
       <c r="F4" s="3">
         <v>750</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>7</v>
@@ -1123,30 +1138,34 @@
       <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
       </c>
       <c r="F5" s="3">
         <v>21000</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
@@ -1157,33 +1176,37 @@
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" s="3">
         <v>160000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>7</v>
@@ -1191,27 +1214,31 @@
       <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="M6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>93</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>94</v>
       </c>
       <c r="F7" s="3">
         <v>650</v>
@@ -1223,32 +1250,36 @@
         <v>7</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="3">
         <v>2000</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>7</v>
@@ -1259,30 +1290,37 @@
       <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="M8" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
         <v>100</v>
       </c>
-      <c r="D9" t="s">
-        <v>101</v>
-      </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3">
-        <v>5000</v>
+        <v>1100</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>7</v>
@@ -1293,21 +1331,25 @@
       <c r="J9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="M9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1319,7 +1361,7 @@
         <v>3800</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>7</v>
@@ -1330,33 +1372,37 @@
       <c r="J10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="M10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" s="3">
         <v>5000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>7</v>
@@ -1367,27 +1413,31 @@
       <c r="J11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="M11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="3">
         <v>200</v>
@@ -1398,21 +1448,22 @@
       <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" t="s">
         <v>114</v>
-      </c>
-      <c r="D13" t="s">
-        <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1420,6 +1471,9 @@
       <c r="F13" s="3">
         <v>4500</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1429,27 +1483,31 @@
       <c r="J13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="M13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" t="s">
         <v>118</v>
-      </c>
-      <c r="D14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" t="s">
-        <v>119</v>
       </c>
       <c r="F14" s="3">
         <v>200</v>
@@ -1463,27 +1521,28 @@
       <c r="J14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="3">
         <v>200</v>
@@ -1494,8 +1553,9 @@
       <c r="J15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H5"/>
@@ -1524,7 +1584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -1536,7 +1596,7 @@
       <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -1546,7 +1606,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -1578,7 +1638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1592,7 +1652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1603,7 +1663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1614,7 +1674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -1638,7 +1698,7 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -1646,7 +1706,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -1678,7 +1738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1692,7 +1752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1703,7 +1763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1714,7 +1774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1726,19 +1786,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G52" sqref="G52"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
@@ -1758,7 +1818,7 @@
     <col min="16" max="16" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1796,27 +1856,27 @@
         <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1834,13 +1894,13 @@
         <v>76418</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>7</v>
@@ -1855,15 +1915,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1881,13 +1941,13 @@
         <v>434246</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>7</v>
@@ -1903,15 +1963,15 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1929,13 +1989,13 @@
         <v>331800</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>7</v>
@@ -1951,15 +2011,15 @@
       </c>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1974,16 +2034,16 @@
         <v>7</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>7</v>
@@ -1998,15 +2058,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -2024,13 +2084,13 @@
         <v>122830</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>7</v>
@@ -2046,15 +2106,15 @@
       </c>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2069,13 +2129,13 @@
         <v>64598</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>7</v>
@@ -2091,15 +2151,15 @@
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -2117,13 +2177,13 @@
         <v>60000</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>7</v>
@@ -2139,21 +2199,21 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>7</v>
@@ -2162,13 +2222,13 @@
         <v>109800</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>7</v>
@@ -2181,15 +2241,15 @@
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -2207,13 +2267,13 @@
         <v>97000</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>7</v>
@@ -2229,21 +2289,21 @@
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>7</v>
@@ -2252,13 +2312,13 @@
         <v>46421</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>7</v>
@@ -2268,15 +2328,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -2291,13 +2351,13 @@
         <v>13800</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>7</v>
@@ -2312,21 +2372,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>7</v>
@@ -2338,7 +2398,7 @@
         <v>7</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>7</v>
@@ -2348,15 +2408,15 @@
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -2374,13 +2434,13 @@
         <v>12000</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>7</v>
@@ -2418,7 +2478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -2430,7 +2490,7 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -2438,7 +2498,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -2470,7 +2530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -2484,7 +2544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -2495,7 +2555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2506,7 +2566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
@@ -2518,7 +2578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -2530,7 +2590,7 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -2538,7 +2598,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -2570,7 +2630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -2584,7 +2644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -2595,7 +2655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2606,7 +2666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
@@ -2618,7 +2678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2630,7 +2690,7 @@
       <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="9" customWidth="1"/>
@@ -2648,7 +2708,7 @@
     <col min="14" max="14" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2680,27 +2740,27 @@
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -2715,15 +2775,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -2738,15 +2798,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -2761,21 +2821,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>7</v>
@@ -2784,15 +2844,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -2807,15 +2867,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2830,38 +2890,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2876,21 +2936,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>7</v>
@@ -2899,21 +2959,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>7</v>
@@ -2922,21 +2982,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>7</v>
@@ -2966,7 +3026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -2978,7 +3038,7 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -2991,7 +3051,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -3002,16 +3062,16 @@
         <v>19</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>8</v>
@@ -3023,18 +3083,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -3045,7 +3105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3056,7 +3116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
@@ -3068,7 +3128,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="1" tint="0.14999847407452621"/>
   </sheetPr>
@@ -3080,7 +3140,7 @@
       <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -3088,7 +3148,7 @@
     <col min="10" max="10" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
@@ -3120,7 +3180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3134,7 +3194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -3145,7 +3205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3156,7 +3216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
start shortlist mobile banking
</commit_message>
<xml_diff>
--- a/03_UE1_Anbieterevaluierung.xlsx
+++ b/03_UE1_Anbieterevaluierung.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="174">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -968,10 +968,10 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C31" sqref="C31"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1138,6 +1138,9 @@
       <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="L4" s="3" t="s">
         <v>168</v>
       </c>
@@ -1174,6 +1177,9 @@
         <v>7</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="3" t="s">

</xml_diff>

<commit_message>
longlist update, shortlist mobile banking finished
</commit_message>
<xml_diff>
--- a/03_UE1_Anbieterevaluierung.xlsx
+++ b/03_UE1_Anbieterevaluierung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="715" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" tabRatio="715"/>
   </bookViews>
   <sheets>
     <sheet name="Mobile Banking" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="181">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -531,13 +531,46 @@
   </si>
   <si>
     <t>DIGIPASS</t>
+  </si>
+  <si>
+    <t>gegründet 1968, weltweit über 14000 Kunden</t>
+  </si>
+  <si>
+    <t>gegründet 1984, unterstützt 1000 Institutionen weltweit</t>
+  </si>
+  <si>
+    <t>gegründet 2003, Dienstleister von 350 Institutionen weltweit</t>
+  </si>
+  <si>
+    <t>gegründet 1981, Hauptsitz in Indien</t>
+  </si>
+  <si>
+    <t>gegründet 1995</t>
+  </si>
+  <si>
+    <t>gegründet 1976, Partner von über 1300 Banken</t>
+  </si>
+  <si>
+    <t>gegründet 2007,  über 20Mil. Nutzer von über 600 Apps</t>
+  </si>
+  <si>
+    <t>Tochter der SAP-Gruppe</t>
+  </si>
+  <si>
+    <t>gegründet 1975, Dienstleister von 1650 Banken und Institutionen</t>
+  </si>
+  <si>
+    <t>gegründet 1963, weltweit über 1800 Kunden</t>
+  </si>
+  <si>
+    <t>gegründet 2005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -719,7 +752,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -754,7 +786,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -930,19 +961,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C31" sqref="C31"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" style="8" customWidth="1"/>
@@ -957,10 +988,10 @@
     <col min="11" max="11" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31.7109375" style="5" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="14" max="14" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1036,8 +1067,9 @@
         <v>5</v>
       </c>
       <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1077,8 +1109,11 @@
       <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1115,8 +1150,11 @@
       <c r="M4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1156,8 +1194,11 @@
       <c r="M5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1197,8 +1238,11 @@
       <c r="M6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1232,8 +1276,11 @@
       <c r="M7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1273,8 +1320,11 @@
       <c r="M8" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1314,8 +1364,11 @@
       <c r="M9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1355,8 +1408,11 @@
       <c r="M10" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1396,8 +1452,11 @@
       <c r="M11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1425,8 +1484,9 @@
       <c r="L12" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1466,8 +1526,11 @@
       <c r="M13" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1501,8 +1564,11 @@
       <c r="L14" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1530,6 +1596,7 @@
       <c r="L15" s="3" t="s">
         <v>141</v>
       </c>
+      <c r="N15" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H5"/>
@@ -1558,7 +1625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
@@ -1570,7 +1637,7 @@
       <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
@@ -1590,7 +1657,7 @@
     <col min="16" max="16" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +1707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1687,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1735,7 +1802,7 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1783,7 +1850,7 @@
       </c>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1830,7 +1897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1878,7 +1945,7 @@
       </c>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1923,7 +1990,7 @@
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1971,7 +2038,7 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -2013,7 +2080,7 @@
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2061,7 +2128,7 @@
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -2100,7 +2167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -2144,7 +2211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2180,7 +2247,7 @@
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -2250,19 +2317,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H52" sqref="H52"/>
       <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" style="8" customWidth="1"/>
@@ -2280,7 +2347,7 @@
     <col min="14" max="14" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -2365,7 +2432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -2406,7 +2473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2441,7 +2508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -2482,7 +2549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -2523,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2559,7 +2626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -2595,7 +2662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -2636,7 +2703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2674,7 +2741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -2712,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="7">
         <v>11</v>
       </c>

</xml_diff>